<commit_message>
fix bug post & btc
</commit_message>
<xml_diff>
--- a/Capstone_SWP490/Capstone_SWP490/App_Data/registration_form.xlsx
+++ b/Capstone_SWP490/Capstone_SWP490/App_Data/registration_form.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20375"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\The Anh\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\Personal\V5\Capstone_SWP490\Capstone_SWP490\Capstone_SWP490\App_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFEE7ABD-B20C-4A2B-B5CE-8E14DCA4F342}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="4" r:id="rId1"/>
@@ -20,7 +19,7 @@
     <sheet name="Contest Information" sheetId="3" r:id="rId5"/>
     <sheet name="Registration Rule" sheetId="5" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -30,12 +29,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>The Anh</author>
   </authors>
   <commentList>
-    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{F7EC664B-93B2-4BEA-BFFD-76517720949B}">
+    <comment ref="C1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -48,7 +47,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C2" authorId="0" shapeId="0" xr:uid="{82AB090B-CBB4-422D-BF5C-CC2358FA0A71}">
+    <comment ref="C2" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -62,7 +61,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C3" authorId="0" shapeId="0" xr:uid="{A6988401-2AB5-4522-AAF5-4E6816923A83}">
+    <comment ref="C3" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -75,7 +74,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C4" authorId="0" shapeId="0" xr:uid="{166B0EC4-CD15-438B-8197-D2E052B15796}">
+    <comment ref="C4" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -88,7 +87,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C5" authorId="0" shapeId="0" xr:uid="{01EA6DCF-CDD1-4901-A736-305BA5A36535}">
+    <comment ref="C5" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -101,7 +100,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C6" authorId="0" shapeId="0" xr:uid="{1C1BB822-2668-4A1C-A0E2-7CC5C6189F8D}">
+    <comment ref="C6" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -114,7 +113,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C7" authorId="0" shapeId="0" xr:uid="{2108F775-6104-4215-9A32-31AEA1FC14A9}">
+    <comment ref="C7" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -127,7 +126,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C8" authorId="0" shapeId="0" xr:uid="{4ED7A30A-48B8-4CAA-A5CB-77A7FA194C12}">
+    <comment ref="C8" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -140,7 +139,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C9" authorId="0" shapeId="0" xr:uid="{CC6B4872-10B3-4285-B496-D3B25EA68B1F}">
+    <comment ref="C9" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -153,7 +152,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C10" authorId="0" shapeId="0" xr:uid="{7EEC9A0E-74D5-4C13-A3FC-0B8316ECFB6F}">
+    <comment ref="C10" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -166,7 +165,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C11" authorId="0" shapeId="0" xr:uid="{10E388AB-51E8-4A36-9AE2-252D43EEDBF6}">
+    <comment ref="C11" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -179,7 +178,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C12" authorId="0" shapeId="0" xr:uid="{6B73728B-BCBD-42FC-8C3D-DFCF1306650C}">
+    <comment ref="C12" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -197,12 +196,12 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>The Anh</author>
   </authors>
   <commentList>
-    <comment ref="C4" authorId="0" shapeId="0" xr:uid="{C5670B03-ACCA-4238-852B-D04F43CAE18F}">
+    <comment ref="C4" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -215,7 +214,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D4" authorId="0" shapeId="0" xr:uid="{8953DE9F-D774-4A2F-B7C3-35A79DD2FA24}">
+    <comment ref="D4" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -228,7 +227,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E4" authorId="0" shapeId="0" xr:uid="{1159F85D-52D9-4B41-9C8E-46A96B82BE44}">
+    <comment ref="E4" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -242,7 +241,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F4" authorId="0" shapeId="0" xr:uid="{05389968-524F-4F98-8881-C08A47B825FF}">
+    <comment ref="F4" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -265,7 +264,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G4" authorId="0" shapeId="0" xr:uid="{A87E08BD-3BE8-439C-9D90-DDE8A7E37C39}">
+    <comment ref="G4" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -283,12 +282,12 @@
 </file>
 
 <file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>The Anh</author>
   </authors>
   <commentList>
-    <comment ref="L1" authorId="0" shapeId="0" xr:uid="{96E18AEE-0536-4A21-9EBD-2C448D28273F}">
+    <comment ref="L1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -301,7 +300,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C3" authorId="0" shapeId="0" xr:uid="{F87B0EF9-F1AC-4492-B896-EFAD2391F6B9}">
+    <comment ref="C3" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -314,7 +313,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D3" authorId="0" shapeId="0" xr:uid="{859D5247-43D1-4DF9-85F7-04890E949343}">
+    <comment ref="D3" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -327,7 +326,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E3" authorId="0" shapeId="0" xr:uid="{765040FC-25DD-4ED6-9CEC-6F24D57EA003}">
+    <comment ref="E3" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -340,7 +339,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F3" authorId="0" shapeId="0" xr:uid="{A5BE9F87-D184-4764-AA8F-26CB5411B972}">
+    <comment ref="F3" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -354,7 +353,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G3" authorId="0" shapeId="0" xr:uid="{C5E54904-ABDC-4D07-A083-CAD26FE67419}">
+    <comment ref="G3" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -367,7 +366,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H3" authorId="0" shapeId="0" xr:uid="{E98957E6-95B3-48D1-ACA0-5490EBE8EB85}">
+    <comment ref="H3" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -380,7 +379,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I3" authorId="0" shapeId="0" xr:uid="{767FF24E-301A-4463-BAC1-68F5F39E6EFA}">
+    <comment ref="I3" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -393,7 +392,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J3" authorId="0" shapeId="0" xr:uid="{31F05844-E48C-418B-94CB-5833AF45AFB9}">
+    <comment ref="J3" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -406,7 +405,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K3" authorId="0" shapeId="0" xr:uid="{7EC23870-74D8-4E70-9285-5F175DD3018A}">
+    <comment ref="K3" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -424,7 +423,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="93">
   <si>
     <t>Team members</t>
   </si>
@@ -618,9 +617,6 @@
     <t>PMNM</t>
   </si>
   <si>
-    <t>Team Contest Name</t>
-  </si>
-  <si>
     <t>Trần Tiến Anh</t>
   </si>
   <si>
@@ -737,11 +733,17 @@
   <si>
     <t>Giải ba cuộc thi ca nhạc</t>
   </si>
+  <si>
+    <t>Team Contest</t>
+  </si>
+  <si>
+    <t>Column Team Contest take contest code refer sheet Contest Information</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -855,7 +857,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
@@ -887,9 +889,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
@@ -898,6 +897,15 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1179,7 +1187,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1214,7 +1222,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1241,7 +1249,7 @@
         <v>45</v>
       </c>
       <c r="C2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.25">
@@ -1281,7 +1289,7 @@
         <v>18</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.25">
@@ -1289,7 +1297,7 @@
         <v>19</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="9" spans="2:3" x14ac:dyDescent="0.25">
@@ -1317,8 +1325,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C6" r:id="rId1" xr:uid="{D2ACE33A-CA77-4BB6-AA1B-F7F23EB4EE52}"/>
-    <hyperlink ref="C8" r:id="rId2" xr:uid="{284086EF-869D-476B-AD26-0CABE11747D6}"/>
+    <hyperlink ref="C6" r:id="rId1"/>
+    <hyperlink ref="C8" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
@@ -1327,11 +1335,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1347,6 +1355,13 @@
       <c r="A1" t="s">
         <v>24</v>
       </c>
+      <c r="B1" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="22"/>
       <c r="G1"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -1357,19 +1372,19 @@
       <c r="G2" s="1"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C3" s="18" t="s">
-        <v>56</v>
-      </c>
-      <c r="D3" s="18" t="s">
+      <c r="C3" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="D3" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="18" t="s">
+      <c r="E3" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="F3" s="18" t="s">
+      <c r="F3" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="18" t="s">
+      <c r="G3" s="17" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1378,13 +1393,13 @@
         <v>26</v>
       </c>
       <c r="D4" t="s">
+        <v>57</v>
+      </c>
+      <c r="E4" t="s">
+        <v>56</v>
+      </c>
+      <c r="F4" s="13" t="s">
         <v>58</v>
-      </c>
-      <c r="E4" t="s">
-        <v>57</v>
-      </c>
-      <c r="F4" s="13" t="s">
-        <v>59</v>
       </c>
       <c r="G4" s="14" t="s">
         <v>50</v>
@@ -1392,35 +1407,36 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F5" s="13" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G5" s="14" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4:C1048576" xr:uid="{C572F136-2807-457A-8A31-7FF2BF30DE04}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4:C1048576">
       <formula1>"PROCON, PMNM,ICPC"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="F4" r:id="rId1" xr:uid="{A7F19D83-B4F5-411A-B249-2865A18476D0}"/>
-    <hyperlink ref="F5" r:id="rId2" xr:uid="{AC0E78FB-0F32-424F-B7DD-BBA13676D4B8}"/>
+    <hyperlink ref="F4" r:id="rId1"/>
+    <hyperlink ref="F5" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
+  <legacyDrawing r:id="rId4"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1455,12 +1471,12 @@
       <c r="I1" s="3"/>
       <c r="J1" s="3"/>
       <c r="K1" s="3"/>
-      <c r="L1" s="17" t="s">
+      <c r="L1" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="M1" s="17"/>
-      <c r="N1" s="17"/>
-      <c r="O1" s="17"/>
+      <c r="M1" s="20"/>
+      <c r="N1" s="20"/>
+      <c r="O1" s="20"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
@@ -1481,7 +1497,7 @@
         <v>6</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I2" s="4" t="s">
         <v>7</v>
@@ -1507,22 +1523,22 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E3" s="5">
         <v>36067</v>
       </c>
       <c r="F3" s="13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G3" s="14" t="s">
         <v>50</v>
       </c>
       <c r="H3" s="14" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I3" t="s">
         <v>11</v>
@@ -1531,7 +1547,7 @@
         <v>5</v>
       </c>
       <c r="K3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="L3" t="s">
         <v>13</v>
@@ -1548,19 +1564,19 @@
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E4" s="5">
         <v>36141</v>
       </c>
       <c r="F4" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="G4" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="H4" s="14" t="s">
         <v>75</v>
-      </c>
-      <c r="G4" s="14" t="s">
-        <v>82</v>
-      </c>
-      <c r="H4" s="14" t="s">
-        <v>76</v>
       </c>
       <c r="I4" t="s">
         <v>11</v>
@@ -1569,7 +1585,7 @@
         <v>5</v>
       </c>
       <c r="K4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="L4" t="s">
         <v>12</v>
@@ -1586,19 +1602,19 @@
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F5" s="13" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G5" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="H5" s="14" t="s">
         <v>83</v>
-      </c>
-      <c r="H5" s="14" t="s">
-        <v>84</v>
       </c>
       <c r="I5" t="s">
         <v>11</v>
@@ -1607,7 +1623,7 @@
         <v>2</v>
       </c>
       <c r="K5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="L5" t="s">
         <v>13</v>
@@ -1624,25 +1640,25 @@
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D6" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="F6" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="F6" s="13" t="s">
+      <c r="G6" s="14" t="s">
         <v>86</v>
       </c>
-      <c r="G6" s="14" t="s">
+      <c r="H6" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="H6" s="14" t="s">
+      <c r="I6" t="s">
         <v>88</v>
-      </c>
-      <c r="I6" t="s">
-        <v>89</v>
       </c>
       <c r="J6">
         <v>3</v>
       </c>
       <c r="K6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="L6" t="s">
         <v>12</v>
@@ -1662,18 +1678,18 @@
     <mergeCell ref="L1:O1"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L3:O1048576" xr:uid="{B4ABF89D-6882-4295-A696-AE0B2B2EAA37}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L3:O1048576">
       <formula1>"yes,no"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I3:I1048576" xr:uid="{58DEBB39-CEA9-4969-9EF0-A70CC8AD7241}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I3:I1048576">
       <formula1>"Male,Female,Other"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="F3" r:id="rId1" xr:uid="{91AF7356-D640-413E-BDB6-FB95D2527E52}"/>
-    <hyperlink ref="F4" r:id="rId2" xr:uid="{7BB935A0-CB61-4B86-9990-8B074375FC02}"/>
-    <hyperlink ref="F5" r:id="rId3" xr:uid="{9AAD482C-3BB9-4BA4-BB3F-058F7B6315FF}"/>
-    <hyperlink ref="F6" r:id="rId4" xr:uid="{AE8D01CB-4480-4981-9A7B-DFD70F71A577}"/>
+    <hyperlink ref="F3" r:id="rId1"/>
+    <hyperlink ref="F4" r:id="rId2"/>
+    <hyperlink ref="F5" r:id="rId3"/>
+    <hyperlink ref="F6" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId5"/>
@@ -1681,7 +1697,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{472BCF9D-140C-4FDC-A787-A7E3C7BBA4B2}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Team!$D$4:$D$996</xm:f>
           </x14:formula1>
@@ -1694,7 +1710,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1717,19 +1733,19 @@
       <c r="E1" s="3"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="C2" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="C2" s="18" t="s">
-        <v>65</v>
-      </c>
-      <c r="D2" s="18" t="s">
+      <c r="D2" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="E2" s="18" t="s">
+      <c r="E2" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="F2" s="18" t="s">
+      <c r="F2" s="17" t="s">
         <v>34</v>
       </c>
     </row>
@@ -1738,7 +1754,7 @@
         <v>39</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D3" s="5">
         <v>44643</v>
@@ -1755,7 +1771,7 @@
         <v>36</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D4" s="5">
         <v>44643</v>
@@ -1772,7 +1788,7 @@
         <v>38</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D5" s="5">
         <v>44643</v>
@@ -1789,7 +1805,7 @@
         <v>10</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D6" s="5">
         <v>44643</v>
@@ -1854,7 +1870,7 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F1048576" xr:uid="{D2CBA346-68A6-4348-B029-6B09546DEBC4}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F1048576">
       <formula1>"Team,Individual"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1864,10 +1880,10 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
@@ -1879,15 +1895,15 @@
   <sheetData>
     <row r="1" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A1" s="16"/>
-      <c r="B1" s="19" t="s">
-        <v>77</v>
+      <c r="B1" s="18" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="19" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1896,7 +1912,7 @@
         <v>42</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -1904,7 +1920,7 @@
         <v>24</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -1912,7 +1928,7 @@
         <v>43</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>

</xml_diff>